<commit_message>
feat：update sword anim change
</commit_message>
<xml_diff>
--- a/battleworld/Excel/Effect_特效表.xlsx
+++ b/battleworld/Excel/Effect_特效表.xlsx
@@ -193,100 +193,100 @@
     <t>单手剑减速特效</t>
   </si>
   <si>
-    <t>-13|0|-17</t>
+    <t>0|0|40</t>
+  </si>
+  <si>
+    <t>#D23030FF</t>
+  </si>
+  <si>
+    <t>单手剑命中特效</t>
+  </si>
+  <si>
+    <t>-6.3|0|-26.88</t>
+  </si>
+  <si>
+    <t>0.9|0.9|1</t>
+  </si>
+  <si>
+    <t>#006FFFFF</t>
+  </si>
+  <si>
+    <t>单手剑加速特效1</t>
+  </si>
+  <si>
+    <t>#006EFFFF</t>
+  </si>
+  <si>
+    <t>单手剑加速特效2</t>
+  </si>
+  <si>
+    <t>#FFCC00FF</t>
+  </si>
+  <si>
+    <t>法师减速</t>
+  </si>
+  <si>
+    <t>法师眩晕特效</t>
+  </si>
+  <si>
+    <t>1|1|1.1</t>
+  </si>
+  <si>
+    <t>#FFCC67FF</t>
+  </si>
+  <si>
+    <t>法师技能8禁锢</t>
+  </si>
+  <si>
+    <t>#FFC14FFF</t>
+  </si>
+  <si>
+    <t>法师技能9减伤</t>
+  </si>
+  <si>
+    <t>#FFCD04FF</t>
+  </si>
+  <si>
+    <t>法师技能10附魔</t>
+  </si>
+  <si>
+    <t>1|1|2</t>
+  </si>
+  <si>
+    <t>#FFCD50FF</t>
+  </si>
+  <si>
+    <t>法师技能10附魔dot</t>
+  </si>
+  <si>
+    <t>1.2|1.2|1.2</t>
+  </si>
+  <si>
+    <t>法师命中特效</t>
+  </si>
+  <si>
+    <t>0|0|20</t>
+  </si>
+  <si>
+    <t>#FFD300FF</t>
+  </si>
+  <si>
+    <t>法师技能4治疗</t>
+  </si>
+  <si>
+    <t>帕姆尼出场特效</t>
+  </si>
+  <si>
+    <t>帕姆尼消失特效</t>
+  </si>
+  <si>
+    <t>10|0|120</t>
+  </si>
+  <si>
+    <t>0|30|-90</t>
   </si>
   <si>
     <t>2.5|2.5|2.5</t>
-  </si>
-  <si>
-    <t>#005ED3FF</t>
-  </si>
-  <si>
-    <t>单手剑命中特效</t>
-  </si>
-  <si>
-    <t>-6.3|0|-26.88</t>
-  </si>
-  <si>
-    <t>0.9|0.9|1</t>
-  </si>
-  <si>
-    <t>#006FFFFF</t>
-  </si>
-  <si>
-    <t>单手剑加速特效1</t>
-  </si>
-  <si>
-    <t>#006EFFFF</t>
-  </si>
-  <si>
-    <t>单手剑加速特效2</t>
-  </si>
-  <si>
-    <t>#FFCC00FF</t>
-  </si>
-  <si>
-    <t>法师减速</t>
-  </si>
-  <si>
-    <t>法师眩晕特效</t>
-  </si>
-  <si>
-    <t>1|1|1.1</t>
-  </si>
-  <si>
-    <t>#FFCC67FF</t>
-  </si>
-  <si>
-    <t>法师技能8禁锢</t>
-  </si>
-  <si>
-    <t>#FFC14FFF</t>
-  </si>
-  <si>
-    <t>法师技能9减伤</t>
-  </si>
-  <si>
-    <t>#FFCD04FF</t>
-  </si>
-  <si>
-    <t>法师技能10附魔</t>
-  </si>
-  <si>
-    <t>1|1|2</t>
-  </si>
-  <si>
-    <t>#FFCD50FF</t>
-  </si>
-  <si>
-    <t>法师技能10附魔dot</t>
-  </si>
-  <si>
-    <t>1.2|1.2|1.2</t>
-  </si>
-  <si>
-    <t>法师命中特效</t>
-  </si>
-  <si>
-    <t>0|0|20</t>
-  </si>
-  <si>
-    <t>#FFD300FF</t>
-  </si>
-  <si>
-    <t>法师技能4治疗</t>
-  </si>
-  <si>
-    <t>帕姆尼出场特效</t>
-  </si>
-  <si>
-    <t>帕姆尼消失特效</t>
-  </si>
-  <si>
-    <t>10|0|120</t>
-  </si>
-  <si>
-    <t>0|30|-90</t>
   </si>
   <si>
     <t>双手剑命中刀光小</t>
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:U181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75"/>
@@ -2026,7 +2026,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3">
-        <v>151736</v>
+        <v>151568</v>
       </c>
       <c r="C14" s="1">
         <v>12</v>
@@ -2038,16 +2038,16 @@
         <v>22</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="4">
-        <v>-0.5</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -2073,22 +2073,22 @@
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G15" s="4">
         <v>-10</v>
       </c>
       <c r="H15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2114,7 +2114,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>22</v>
@@ -2126,10 +2126,10 @@
         <v>-10</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -2167,10 +2167,10 @@
         <v>-2</v>
       </c>
       <c r="H17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -2211,7 +2211,7 @@
         <v>25</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -2243,16 +2243,16 @@
         <v>22</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19" s="4">
         <v>-3</v>
       </c>
       <c r="H19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -2290,10 +2290,10 @@
         <v>-8</v>
       </c>
       <c r="H20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -2331,10 +2331,10 @@
         <v>-8</v>
       </c>
       <c r="H21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -2366,16 +2366,16 @@
         <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G22" s="4">
         <v>-1</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2407,14 +2407,14 @@
         <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G23" s="4">
         <v>-1</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -2440,7 +2440,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>22</v>
@@ -2452,10 +2452,10 @@
         <v>-1</v>
       </c>
       <c r="H24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -2487,14 +2487,14 @@
         <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G25" s="4">
         <v>-2</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -2559,13 +2559,13 @@
         <v>23</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="G27" s="4">
         <v>-1</v>
@@ -2585,7 +2585,7 @@
         <v>23</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>76</v>

</xml_diff>